<commit_message>
clean up raw data
</commit_message>
<xml_diff>
--- a/R_C14_rates calculation/0_data_used/MD FCM DATA_v1.1.xlsx
+++ b/R_C14_rates calculation/0_data_used/MD FCM DATA_v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deniseong/Documents/GitHub/TAN1810_C14/R_C14_rates calculation/0_data_used/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0857E536-09F6-0443-A787-F3B90719A4FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F134B5-A3CF-E14F-9CFE-3D84349EF1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="-100" windowWidth="30340" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="86">
   <si>
     <t>SYN/ML</t>
   </si>
@@ -438,10 +438,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -707,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC5DDA2-8349-0A49-9827-00F853CE3BBF}">
-  <dimension ref="A1:AP206"/>
+  <dimension ref="A1:AP203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="F208" sqref="F208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6126,91 +6122,30 @@
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="C201" s="13"/>
+      <c r="G201" s="3"/>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A202" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="B202" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C202" s="13">
-        <v>43410</v>
+        <v>85</v>
       </c>
       <c r="D202" s="3">
         <v>2</v>
       </c>
-      <c r="E202" s="3">
-        <v>188</v>
-      </c>
       <c r="F202" s="3">
         <v>12</v>
       </c>
-      <c r="G202" s="8">
-        <v>47568.75</v>
-      </c>
-      <c r="H202" s="8">
-        <v>9174.4360902255648</v>
-      </c>
-      <c r="I202" s="8">
-        <v>1843.6090225563912</v>
+      <c r="G202" s="3">
+        <v>74416.875</v>
+      </c>
+      <c r="H202" s="3">
+        <v>10447.072059711323</v>
+      </c>
+      <c r="I202" s="3">
+        <v>2553.9212995993639</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A203" t="s">
-        <v>25</v>
-      </c>
-      <c r="B203" t="s">
-        <v>77</v>
-      </c>
-      <c r="C203" s="13">
-        <v>43408</v>
-      </c>
-      <c r="D203" s="3">
-        <v>2</v>
-      </c>
-      <c r="E203" s="3">
-        <v>159</v>
-      </c>
-      <c r="F203" s="3">
-        <v>12</v>
-      </c>
-      <c r="G203" s="8">
-        <v>101264.99999999999</v>
-      </c>
-      <c r="H203" s="8">
-        <v>11719.708029197081</v>
-      </c>
-      <c r="I203" s="8">
-        <v>3264.2335766423362</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="G204" s="3"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B205" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D205" s="3">
-        <v>2</v>
-      </c>
-      <c r="F205" s="3">
-        <v>12</v>
-      </c>
-      <c r="G205" s="3">
-        <v>74416.875</v>
-      </c>
-      <c r="H205" s="3">
-        <v>10447.072059711323</v>
-      </c>
-      <c r="I205" s="3">
-        <v>2553.9212995993639</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="G206" s="3"/>
+      <c r="G203" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>